<commit_message>
Know-27 Q-Handbuch aktualisiert; Maßnahmenliste hinzugefügt; Checkliste Projekt aktualisiert
</commit_message>
<xml_diff>
--- a/docs/documentation/Qualitätsmanagement/Checklisten/Checkliste Projekt.xlsx
+++ b/docs/documentation/Qualitätsmanagement/Checklisten/Checkliste Projekt.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isa\Documents\Hochschule\Master\docs\documentation\Qualitätsmanagement\Checklisten\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="24240" windowHeight="12330"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
   <si>
     <t>Projektinitiierung</t>
   </si>
@@ -464,14 +469,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -509,9 +517,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -546,7 +554,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -581,7 +589,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -757,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1054,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.25">
@@ -1054,7 +1062,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.25">
@@ -1062,7 +1070,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.25">
@@ -1070,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.25">
@@ -1078,7 +1086,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:47" x14ac:dyDescent="0.25">
@@ -1086,7 +1094,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -1094,7 +1102,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -1102,7 +1110,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -1119,33 +1127,41 @@
       <c r="B21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
@@ -1161,51 +1177,65 @@
       <c r="B28" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
@@ -1221,31 +1251,41 @@
       <c r="B38" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="5"/>
+      <c r="C39" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="5"/>
+      <c r="C40" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
@@ -1261,25 +1301,33 @@
       <c r="B45" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="5"/>
+      <c r="C45" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="5"/>
+      <c r="C47" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="5"/>
+      <c r="C48" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
@@ -1293,19 +1341,25 @@
       <c r="B50" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="5"/>
+      <c r="C51" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>

</xml_diff>